<commit_message>
user-data on Register_login page
</commit_message>
<xml_diff>
--- a/TODO.xlsx
+++ b/TODO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Personal\Abdulrahman\WorkStudy\Courses\Playwright\Automation Eaxercise\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09164529-BCDA-4F63-B144-8C252C1224B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DF4AE28-5B00-466C-B1FE-DE4AD5542F9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>put all error messages in one file</t>
   </si>
@@ -43,16 +43,48 @@
   </si>
   <si>
     <t>solution</t>
+  </si>
+  <si>
+    <t>messages file</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="9"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>applied on register_login page</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> | apply on regesteration page</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="9"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -370,13 +402,13 @@
   <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="33.6640625" customWidth="1"/>
-    <col min="2" max="2" width="48.21875" customWidth="1"/>
+    <col min="2" max="2" width="61.21875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
@@ -388,6 +420,14 @@
       <c r="A2" t="s">
         <v>1</v>
       </c>
+      <c r="B2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">

</xml_diff>